<commit_message>
Update 20180925 - optiqueDesTissus/dataOtptiqueDesTissus.xlsx
</commit_message>
<xml_diff>
--- a/20180925 - optiqueDesTissus/dataOtptiqueDesTissus.xlsx
+++ b/20180925 - optiqueDesTissus/dataOtptiqueDesTissus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnau\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arnau\Documents\GitHub\TPOBLabs\20180925 - optiqueDesTissus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4240D7EC-462F-48B0-8B6D-098854141946}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8916939C-E3E8-44EA-9B56-91EB019C126B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24669" windowHeight="9437" xr2:uid="{7407E724-DB74-49A8-AC87-87D60124024B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>tot</t>
   </si>
@@ -64,6 +64,36 @@
   </si>
   <si>
     <t>abérrantes</t>
+  </si>
+  <si>
+    <t>semaine 2</t>
+  </si>
+  <si>
+    <t>avec correction</t>
+  </si>
+  <si>
+    <t>sans correction</t>
+  </si>
+  <si>
+    <t>transmitance</t>
+  </si>
+  <si>
+    <t>Réflectance</t>
+  </si>
+  <si>
+    <t>tramsitance</t>
+  </si>
+  <si>
+    <t>réflectance</t>
+  </si>
+  <si>
+    <t>absorption (mm^-1)</t>
+  </si>
+  <si>
+    <t>diffusion (mm^-1)</t>
+  </si>
+  <si>
+    <t>diffusion reduce (mm^-1)</t>
   </si>
 </sst>
 </file>
@@ -71,7 +101,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -139,7 +169,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -455,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BAE80F-EC59-4853-9D9D-E280FBDD54E7}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" topLeftCell="C6" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -468,8 +498,11 @@
     <col min="4" max="4" width="12.765625" customWidth="1"/>
     <col min="5" max="5" width="20.3046875" customWidth="1"/>
     <col min="6" max="6" width="19.61328125" customWidth="1"/>
-    <col min="7" max="7" width="18.15234375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.15234375" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.3046875" customWidth="1"/>
+    <col min="10" max="10" width="22.3046875" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="12" max="12" width="28.3046875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
@@ -1434,7 +1467,7 @@
         <v>8.6259999999999994</v>
       </c>
     </row>
-    <row r="33" spans="6:10" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.4">
       <c r="F33" t="s">
         <v>9</v>
       </c>
@@ -1443,7 +1476,7 @@
         <v>2.193199666666666E-4</v>
       </c>
       <c r="H33" s="2">
-        <f t="shared" ref="H33:I33" si="2">AVERAGEA(H2:H31)</f>
+        <f t="shared" ref="H33" si="2">AVERAGEA(H2:H31)</f>
         <v>6.4913433333333339</v>
       </c>
       <c r="I33" s="2">
@@ -1454,7 +1487,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="6:10" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.4">
       <c r="G34" s="2">
         <f>G33*10</f>
         <v>2.1931996666666662E-3</v>
@@ -1469,6 +1502,99 @@
       </c>
       <c r="J34" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F37" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C38" s="2">
+        <v>0.28639999999999999</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.1898</v>
+      </c>
+      <c r="H38">
+        <v>0.3004</v>
+      </c>
+      <c r="I38">
+        <v>0.19320000000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="C39" s="2">
+        <f>C38/(C38+D38)</f>
+        <v>0.60142797144057125</v>
+      </c>
+      <c r="D39" s="2">
+        <f>D38/(D38/C38)</f>
+        <v>0.28639999999999999</v>
+      </c>
+      <c r="E39" s="2">
+        <v>6.0970000000000003E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>9.6843000000000004</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1.2270000000000001</v>
+      </c>
+      <c r="H39">
+        <f>H38/(H38+I38)</f>
+        <v>0.60858995137763372</v>
+      </c>
+      <c r="I39">
+        <f>I38/(H38+I38)</f>
+        <v>0.39141004862236628</v>
+      </c>
+      <c r="J39" s="2">
+        <v>1.2459999999999999E-5</v>
+      </c>
+      <c r="K39" s="2">
+        <v>9.7456999999999994</v>
+      </c>
+      <c r="L39" s="2">
+        <v>1.8009999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>